<commit_message>
Add calculations for parallactic angle.
</commit_message>
<xml_diff>
--- a/data/deltat.xlsx
+++ b/data/deltat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wim/GitHub/laravel-astronomy-library/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81E2592-2DD8-6C40-8A18-846E53F558C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1974BC-C511-D544-8333-EB9E30DE5A39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40340" yWindow="3120" windowWidth="26120" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45360" yWindow="460" windowWidth="26120" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -1571,7 +1571,7 @@
                   <c:v>66.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>66.33</c:v>
+                  <c:v>66.319999999999993</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>66.069999999999993</c:v>
@@ -4045,7 +4045,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" sqref="A1:XFD1"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4139,7 +4139,7 @@
         <v>2011</v>
       </c>
       <c r="B11" s="6">
-        <v>66.33</v>
+        <v>66.319999999999993</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>